<commit_message>
means testing updated to contain group, CIs and NAs
</commit_message>
<xml_diff>
--- a/ph_statistical_methods/tests/test_data/testdata_Mean.xlsx
+++ b/ph_statistical_methods/tests/test_data/testdata_Mean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annabel.Westermann\Documents\Python\Projects\PH_statistical_methods\ph_statistical_methods\tests\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.Stewart_DHSC\Documents\Python\Projects\PH_statistical_methods\ph_statistical_methods\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8661B1-6581-45F9-8B47-00F190EAEE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501E0AA5-C5CA-467F-94CE-4409317A0861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="2790" windowWidth="14400" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Mean" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>Area1</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>upper_99_8_ci</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,12 +656,24 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -670,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated test_2ci and test_NAs to run properly
</commit_message>
<xml_diff>
--- a/ph_statistical_methods/tests/test_data/testdata_Mean.xlsx
+++ b/ph_statistical_methods/tests/test_data/testdata_Mean.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.Stewart_DHSC\Documents\Python\Projects\PH_statistical_methods\ph_statistical_methods\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501E0AA5-C5CA-467F-94CE-4409317A0861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B3C505-EC7C-4A6F-9D6B-0D51303EDA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2790" windowWidth="14400" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="8340" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Mean" sheetId="3" r:id="rId1"/>
     <sheet name="testdata_Mean_results" sheetId="4" r:id="rId2"/>
+    <sheet name="testdata_Mean_results_NA" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="18">
   <si>
     <t>Area1</t>
   </si>
@@ -425,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,16 +665,8 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -845,4 +838,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D913A633-1F17-48BF-AFB1-BB738FAA00D6}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>102221.33323999999</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2117.8317161590671</v>
+      </c>
+      <c r="E3">
+        <v>5678.9629577777778</v>
+      </c>
+      <c r="F3">
+        <v>4625.7900224529722</v>
+      </c>
+      <c r="G3">
+        <v>6732.1358931025834</v>
+      </c>
+      <c r="H3">
+        <v>3859.0770997295967</v>
+      </c>
+      <c r="I3">
+        <v>7498.8488158259588</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B2:B3)</f>
+        <v>102221.33323999999</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>3171.8018122194453</v>
+      </c>
+      <c r="E4">
+        <v>3948.1141538461534</v>
+      </c>
+      <c r="F4">
+        <v>2666.9956767458489</v>
+      </c>
+      <c r="G4">
+        <v>5229.2326309464579</v>
+      </c>
+      <c r="H4">
+        <v>1801.9535385474737</v>
+      </c>
+      <c r="I4">
+        <v>6094.274769144833</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test data and ran suitable tests. Fixed test scripts in test_means.
</commit_message>
<xml_diff>
--- a/ph_statistical_methods/tests/test_data/testdata_Mean.xlsx
+++ b/ph_statistical_methods/tests/test_data/testdata_Mean.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annabel.Westermann\Documents\Python\Projects\PH_statistical_methods\ph_statistical_methods\tests\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.Stewart_DHSC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8661B1-6581-45F9-8B47-00F190EAEE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{616B596E-9955-4DEE-A59D-0B26E30E719B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Mean" sheetId="3" r:id="rId1"/>
     <sheet name="testdata_Mean_results" sheetId="4" r:id="rId2"/>
+    <sheet name="testdata_Mean_results_NA" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="18">
   <si>
     <t>Area1</t>
   </si>
@@ -88,6 +89,9 @@
   </si>
   <si>
     <t>upper_99_8_ci</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -425,18 +429,18 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -444,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -452,7 +456,7 @@
         <v>33.09375</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -460,7 +464,7 @@
         <v>48.385959999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,7 +472,7 @@
         <v>64.834950000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,7 +480,7 @@
         <v>67.984750000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -484,7 +488,7 @@
         <v>22.935559999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -492,7 +496,7 @@
         <v>71.235870000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -500,7 +504,7 @@
         <v>38.784649999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,7 +512,7 @@
         <v>82.379270000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -516,7 +520,7 @@
         <v>5555.6666599999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -524,7 +528,7 @@
         <v>6666.7777699999997</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -532,7 +536,7 @@
         <v>4444.8888800000004</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -540,7 +544,7 @@
         <v>2222.9999899999998</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -548,7 +552,7 @@
         <v>3333.88888</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -556,7 +560,7 @@
         <v>5555.4444400000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -564,7 +568,7 @@
         <v>6666.3333300000004</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -572,7 +576,7 @@
         <v>7777.4444400000002</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -580,7 +584,7 @@
         <v>5555.9999900000003</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -588,7 +592,7 @@
         <v>8888.3333299999995</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -596,7 +600,7 @@
         <v>2222.55555</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -604,7 +608,7 @@
         <v>4444.3333300000004</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -612,7 +616,7 @@
         <v>6666.2222199999997</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -620,7 +624,7 @@
         <v>4444.1111099999998</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
@@ -628,7 +632,7 @@
         <v>4444.2222199999997</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -636,7 +640,7 @@
         <v>5555.1111099999998</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
@@ -644,7 +648,7 @@
         <v>7777.2222199999997</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -652,11 +656,15 @@
         <v>9999.7777700000006</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
     </row>
@@ -670,21 +678,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" customWidth="1"/>
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -719,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -754,7 +762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -789,13 +797,179 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <f>SUM(B2:B3)</f>
         <v>102650.96799999999</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>3171.8018122194453</v>
+      </c>
+      <c r="E4">
+        <v>3948.1141538461534</v>
+      </c>
+      <c r="F4">
+        <v>2666.9956767458489</v>
+      </c>
+      <c r="G4">
+        <v>5229.2326309464579</v>
+      </c>
+      <c r="H4">
+        <v>1801.9535385474737</v>
+      </c>
+      <c r="I4">
+        <v>6094.274769144833</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D913A633-1F17-48BF-AFB1-BB738FAA00D6}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>102221.33323999999</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2117.8317161590671</v>
+      </c>
+      <c r="E3">
+        <v>5678.9629577777778</v>
+      </c>
+      <c r="F3">
+        <v>4625.7900224529722</v>
+      </c>
+      <c r="G3">
+        <v>6732.1358931025834</v>
+      </c>
+      <c r="H3">
+        <v>3859.0770997295967</v>
+      </c>
+      <c r="I3">
+        <v>7498.8488158259588</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B2:B3)</f>
+        <v>102221.33323999999</v>
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>

</xml_diff>